<commit_message>
Added signup data for tests
</commit_message>
<xml_diff>
--- a/src/main/java/pchub/utilities/ExcelSheet.xlsx
+++ b/src/main/java/pchub/utilities/ExcelSheet.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="SignUp" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t xml:space="preserve">Email Address</t>
   </si>
@@ -28,31 +29,106 @@
     <t xml:space="preserve">Password</t>
   </si>
   <si>
-    <t xml:space="preserve">User</t>
-  </si>
-  <si>
     <t xml:space="preserve">Daisy</t>
   </si>
   <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
     <t xml:space="preserve">daisy@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">password</t>
   </si>
   <si>
-    <t xml:space="preserve">S</t>
-  </si>
-  <si>
     <t xml:space="preserve">nomane@noname.com</t>
   </si>
   <si>
     <t xml:space="preserve">No’password</t>
   </si>
   <si>
-    <t xml:space="preserve">V</t>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NickName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email Conf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passconf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Info</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>daisy#@gm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>.com</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">fdsaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newpassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dsbas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asfadfa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cameroon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://gmail.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdfs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">passconf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dsfa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">daisy@yagm.com</t>
   </si>
 </sst>
 </file>
@@ -67,6 +143,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -88,12 +165,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -168,18 +247,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5612244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -189,41 +268,29 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -239,4 +306,189 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.969387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.6683673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5612244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.280612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6173469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5612244897959"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.8367346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.4183673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" location="@gm" display="daisy#@gm"/>
+    <hyperlink ref="J2" r:id="rId2" display="http://gmail.com/"/>
+    <hyperlink ref="C4" r:id="rId3" display="daisy@yagm.com"/>
+    <hyperlink ref="D4" r:id="rId4" display="daisy@yagm.com"/>
+    <hyperlink ref="J4" r:id="rId5" display="http://gmail.com/"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added email address data for the 'Forgot Password' functionality
</commit_message>
<xml_diff>
--- a/src/main/java/pchub/utilities/ExcelSheet.xlsx
+++ b/src/main/java/pchub/utilities/ExcelSheet.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="SignUp" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="SignInPage" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
   <si>
     <t xml:space="preserve">Email Address</t>
   </si>
@@ -141,6 +142,9 @@
   </si>
   <si>
     <t xml:space="preserve">Some Info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emailaddress@yahoo.fr</t>
   </si>
 </sst>
 </file>
@@ -262,15 +266,14 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -336,22 +339,24 @@
   </sheetPr>
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.02551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -580,4 +585,68 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="emailaddress@yahoo.fr"/>
+    <hyperlink ref="A3" r:id="rId2" display="nomane@noname.com"/>
+    <hyperlink ref="A4" r:id="rId3" display="daisy@yagm.com"/>
+    <hyperlink ref="A6" r:id="rId4" display="daisy@yagm.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>